<commit_message>
Updated religion and race
</commit_message>
<xml_diff>
--- a/elsa/G2A ELSA Family Variable List.xlsx
+++ b/elsa/G2A ELSA Family Variable List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09B709A-F7F7-42A8-83A9-F1C786EA9E78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C04385F-03A0-4A12-A9D6-5485900718E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22310" yWindow="2810" windowWidth="19260" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -882,7 +882,127 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1272,8 +1392,8 @@
   <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2351,36 +2471,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B90:B1048576 B74:B85 B14:B19 B30:B65 B21:B28 B1:B12">
-    <cfRule type="duplicateValues" dxfId="10" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:E6 F4 D3 E3:E4">
-    <cfRule type="duplicateValues" dxfId="7" priority="106"/>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E20">
-    <cfRule type="duplicateValues" dxfId="6" priority="109"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E62:E65">
-    <cfRule type="duplicateValues" dxfId="5" priority="110"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
-    <cfRule type="duplicateValues" dxfId="4" priority="139"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D52:E53">
-    <cfRule type="duplicateValues" dxfId="3" priority="146"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
-    <cfRule type="duplicateValues" dxfId="2" priority="219"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E61 D40:E42 D15:E15 D45:E45 D58:E58 D61:D65">
-    <cfRule type="duplicateValues" dxfId="1" priority="240"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57:E57">
+  <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revised commit after excluding strata variable and imputing sample weights
</commit_message>
<xml_diff>
--- a/elsa/G2A ELSA Family Variable List.xlsx
+++ b/elsa/G2A ELSA Family Variable List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C04385F-03A0-4A12-A9D6-5485900718E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7311E86B-5CB0-4102-885F-0071482F1361}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22310" yWindow="2810" windowWidth="19260" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -882,187 +882,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1392,8 +1212,8 @@
   <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2471,16 +2291,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B90:B1048576 B74:B85 B14:B19 B30:B65 B21:B28 B1:B12">
-    <cfRule type="duplicateValues" dxfId="8" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="7" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>

<commit_message>
Added summary table for ELSA with spouse-specific sample weights
</commit_message>
<xml_diff>
--- a/elsa/G2A ELSA Family Variable List.xlsx
+++ b/elsa/G2A ELSA Family Variable List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7311E86B-5CB0-4102-885F-0071482F1361}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99DDFF4-4E16-4B83-BD77-5FF5FD0EF80D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22310" yWindow="2810" windowWidth="19260" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="261">
   <si>
     <t>BMI</t>
   </si>
@@ -792,6 +792,18 @@
   </si>
   <si>
     <t>s8mweight</t>
+  </si>
+  <si>
+    <t>Wave-specific cohort category</t>
+  </si>
+  <si>
+    <t>cohort</t>
+  </si>
+  <si>
+    <t>r8cohort_e</t>
+  </si>
+  <si>
+    <t>s8cohort_e</t>
   </si>
 </sst>
 </file>
@@ -1209,11 +1221,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{271C18A0-0761-4BF3-9F1D-A36E2FCBDA0F}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1352,13 +1364,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>257</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>258</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -1366,16 +1384,10 @@
         <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>190</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -1383,16 +1395,16 @@
         <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>125</v>
+        <v>190</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -1400,16 +1412,16 @@
         <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>111</v>
+        <v>60</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1417,16 +1429,16 @@
         <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>191</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1434,33 +1446,30 @@
         <v>62</v>
       </c>
       <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
         <v>95</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>96</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>193</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1468,19 +1477,19 @@
         <v>77</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>237</v>
+        <v>146</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -1488,53 +1497,56 @@
         <v>77</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>148</v>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1542,56 +1554,53 @@
         <v>77</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>86</v>
+        <v>121</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>74</v>
+        <v>122</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -1599,19 +1608,19 @@
         <v>77</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>115</v>
+        <v>74</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -1619,16 +1628,16 @@
         <v>77</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>30</v>
+        <v>114</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>133</v>
@@ -1639,119 +1648,119 @@
         <v>77</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="7" t="s">
+      <c r="A25" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C26" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D26" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E26" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F26" s="8" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>251</v>
-      </c>
+      <c r="B27" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="B28" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
         <v>161</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>162</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -1759,16 +1768,16 @@
         <v>77</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>196</v>
@@ -1778,51 +1787,54 @@
       <c r="A32" t="s">
         <v>77</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>166</v>
+      <c r="B32" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>77</v>
       </c>
-      <c r="B33" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>234</v>
+      <c r="B33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>181</v>
+      <c r="B34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -1830,16 +1842,16 @@
         <v>77</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -1847,16 +1859,16 @@
         <v>77</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -1864,16 +1876,16 @@
         <v>77</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -1881,16 +1893,16 @@
         <v>77</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -1898,33 +1910,33 @@
         <v>77</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>77</v>
       </c>
-      <c r="B40" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40" t="s">
-        <v>89</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>187</v>
+      <c r="B40" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -1932,16 +1944,16 @@
         <v>77</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -1949,10 +1961,16 @@
         <v>77</v>
       </c>
       <c r="B42" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C42" t="s">
-        <v>92</v>
+        <v>90</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -1960,27 +1978,21 @@
         <v>77</v>
       </c>
       <c r="B43" t="s">
-        <v>18</v>
+        <v>91</v>
       </c>
       <c r="C43" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>228</v>
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
@@ -1988,27 +2000,33 @@
         <v>77</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>77</v>
       </c>
-      <c r="B46" t="s">
-        <v>78</v>
-      </c>
-      <c r="C46" t="s">
-        <v>82</v>
+      <c r="B46" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
@@ -2016,10 +2034,10 @@
         <v>77</v>
       </c>
       <c r="B47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
@@ -2027,10 +2045,10 @@
         <v>77</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="C48" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -2038,10 +2056,10 @@
         <v>77</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C49" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
@@ -2049,10 +2067,10 @@
         <v>77</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
@@ -2060,27 +2078,21 @@
         <v>77</v>
       </c>
       <c r="B51" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>77</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>226</v>
+      <c r="B52" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
@@ -2088,27 +2100,33 @@
         <v>77</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>77</v>
       </c>
-      <c r="B54" t="s">
-        <v>80</v>
-      </c>
-      <c r="C54" t="s">
-        <v>84</v>
+      <c r="B54" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
@@ -2116,10 +2134,10 @@
         <v>77</v>
       </c>
       <c r="B55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C55" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
@@ -2127,10 +2145,10 @@
         <v>77</v>
       </c>
       <c r="B56" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="C56" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
@@ -2138,16 +2156,10 @@
         <v>77</v>
       </c>
       <c r="B57" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C57" t="s">
-        <v>71</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>256</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
@@ -2155,33 +2167,33 @@
         <v>77</v>
       </c>
       <c r="B58" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C58" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>223</v>
+        <v>255</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>224</v>
+        <v>256</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>77</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>232</v>
+      <c r="B59" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59" t="s">
+        <v>72</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -2189,36 +2201,36 @@
         <v>77</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>241</v>
+        <v>73</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>61</v>
-      </c>
-      <c r="B61" t="s">
-        <v>32</v>
-      </c>
-      <c r="C61" t="s">
-        <v>119</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>221</v>
+        <v>77</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>243</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>222</v>
+        <v>244</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
@@ -2226,16 +2238,16 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C62" t="s">
-        <v>117</v>
-      </c>
-      <c r="D62" t="s">
-        <v>245</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>245</v>
+        <v>119</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
@@ -2243,16 +2255,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>108</v>
+        <v>33</v>
       </c>
       <c r="C63" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D63" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
@@ -2260,43 +2272,60 @@
         <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C64" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D64" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>61</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" t="s">
+        <v>109</v>
+      </c>
+      <c r="C65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D65" t="s">
+        <v>247</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>61</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C66" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D65" s="6" t="s">
+      <c r="D66" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="E65" s="6" t="s">
+      <c r="E66" s="6" t="s">
         <v>173</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B90:B1048576 B74:B85 B14:B19 B30:B65 B21:B28 B1:B12">
+  <conditionalFormatting sqref="B91:B1048576 B75:B86 B15:B20 B31:B66 B22:B29 B1:B13">
     <cfRule type="duplicateValues" dxfId="4" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
+  <conditionalFormatting sqref="B14">
     <cfRule type="duplicateValues" dxfId="3" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
+  <conditionalFormatting sqref="B21">
     <cfRule type="duplicateValues" dxfId="2" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">

</xml_diff>